<commit_message>
Results from July 18, 2020 08:53:55 AM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-18.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-18.xlsx
@@ -1644,21 +1644,39 @@
           <t>Kansas</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
+      <c r="B25" s="2" t="n">
+        <v>44029</v>
+      </c>
+      <c r="C25" t="n">
+        <v>21965</v>
+      </c>
+      <c r="D25" t="n">
+        <v>299</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1644</v>
+      </c>
+      <c r="F25" t="n">
+        <v>64</v>
+      </c>
+      <c r="G25" t="n">
+        <v>9.18</v>
+      </c>
+      <c r="H25" t="n">
+        <v>21.99</v>
+      </c>
       <c r="I25" t="b">
         <v>0</v>
       </c>
       <c r="J25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K25" t="n">
+        <v>17913</v>
+      </c>
+      <c r="L25" t="n">
+        <v>291</v>
+      </c>
       <c r="M25" t="n">
         <v>169801</v>
       </c>
@@ -1667,7 +1685,7 @@
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>An error occurred. ... WebDriverException('unknown error: Chrome failed to start: exited abnormally.\n  (chrome not reachable)\n  (The process started from chrome location /usr/bin/google-chrome is no longer running, so ChromeDriver is assuming that Chrome has crashed.)', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 18, 2020 07:44:58 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-18.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-18.xlsx
@@ -522,25 +522,25 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C2" t="n">
-        <v>27428</v>
+        <v>27987</v>
       </c>
       <c r="D2" t="n">
-        <v>740</v>
+        <v>749</v>
       </c>
       <c r="E2" t="n">
-        <v>3129</v>
+        <v>3222</v>
       </c>
       <c r="F2" t="n">
         <v>95</v>
       </c>
       <c r="G2" t="n">
-        <v>11.41</v>
+        <v>11.51</v>
       </c>
       <c r="H2" t="n">
-        <v>12.84</v>
+        <v>12.68</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -569,13 +569,13 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C3" t="n">
-        <v>27525</v>
+        <v>28633</v>
       </c>
       <c r="D3" t="n">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="E3" t="n">
         <v>464</v>
@@ -620,26 +620,26 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>217562</t>
+          <t>217895</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18758</t>
+          <t>18771</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>33649</v>
+        <v>33686</v>
       </c>
       <c r="F4" t="n">
-        <v>5246</v>
+        <v>5251</v>
       </c>
       <c r="G4" t="n">
-        <v>30.12</v>
+        <v>30.1</v>
       </c>
       <c r="H4" t="n">
         <v>30.49</v>
@@ -651,10 +651,10 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>111730</v>
+        <v>111896</v>
       </c>
       <c r="L4" t="n">
-        <v>17207</v>
+        <v>17221</v>
       </c>
       <c r="M4" t="n">
         <v>2049418</v>
@@ -773,25 +773,25 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C7" t="n">
-        <v>73819</v>
+        <v>76336</v>
       </c>
       <c r="D7" t="n">
-        <v>815</v>
+        <v>838</v>
       </c>
       <c r="E7" t="n">
-        <v>14737</v>
+        <v>15111</v>
       </c>
       <c r="F7" t="n">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="G7" t="n">
-        <v>19.96</v>
+        <v>19.8</v>
       </c>
       <c r="H7" t="n">
-        <v>35.46</v>
+        <v>35.8</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -820,32 +820,34 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>32572</t>
+          <t>33332</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>235</t>
+          <t>243</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>810</t>
+          <t>830</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>&lt;5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G8" t="n">
         <v>2.5</v>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>1.23</v>
+      </c>
       <c r="I8" t="b">
         <v>1</v>
       </c>
@@ -873,25 +875,25 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C9" t="n">
-        <v>21605</v>
+        <v>22184</v>
       </c>
       <c r="D9" t="n">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="E9" t="n">
-        <v>1908</v>
+        <v>2343</v>
       </c>
       <c r="F9" t="n">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="G9" t="n">
-        <v>12.64</v>
+        <v>15.49</v>
       </c>
       <c r="H9" t="n">
-        <v>14.8</v>
+        <v>4.2</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -900,10 +902,10 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>15097</v>
+        <v>15127</v>
       </c>
       <c r="L9" t="n">
-        <v>615</v>
+        <v>622</v>
       </c>
       <c r="M9" t="n">
         <v>354112</v>
@@ -927,22 +929,22 @@
         <v>44030</v>
       </c>
       <c r="C10" t="n">
-        <v>31762</v>
+        <v>32533</v>
       </c>
       <c r="D10" t="n">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="E10" t="n">
-        <v>6784</v>
+        <v>6918</v>
       </c>
       <c r="F10" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G10" t="n">
         <v>24.53</v>
       </c>
       <c r="H10" t="n">
-        <v>26.29</v>
+        <v>26.2</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -951,10 +953,10 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>27661</v>
+        <v>28197</v>
       </c>
       <c r="L10" t="n">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="M10" t="n">
         <v>460970</v>
@@ -975,25 +977,25 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C11" t="n">
-        <v>22489</v>
+        <v>23114</v>
       </c>
       <c r="D11" t="n">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="E11" t="n">
-        <v>832</v>
+        <v>847</v>
       </c>
       <c r="F11" t="n">
         <v>18</v>
       </c>
       <c r="G11" t="n">
-        <v>4.72</v>
+        <v>4.68</v>
       </c>
       <c r="H11" t="n">
-        <v>3.94</v>
+        <v>3.9</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
@@ -1002,10 +1004,10 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>17636</v>
+        <v>18089</v>
       </c>
       <c r="L11" t="n">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="M11" t="n">
         <v>166412</v>
@@ -1073,16 +1075,16 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C13" t="n">
-        <v>16456</v>
+        <v>16736</v>
       </c>
       <c r="D13" t="n">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="E13" t="n">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
@@ -1206,25 +1208,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C16" t="n">
-        <v>62111</v>
+        <v>64180</v>
       </c>
       <c r="D16" t="n">
-        <v>1232</v>
+        <v>1253</v>
       </c>
       <c r="E16" t="n">
-        <v>19053</v>
+        <v>19494</v>
       </c>
       <c r="F16" t="n">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="G16" t="n">
-        <v>44</v>
+        <v>43.92</v>
       </c>
       <c r="H16" t="n">
-        <v>45.01</v>
+        <v>44.67</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1233,10 +1235,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>43301</v>
+        <v>44381</v>
       </c>
       <c r="L16" t="n">
-        <v>1182</v>
+        <v>1200</v>
       </c>
       <c r="M16" t="n">
         <v>1293186</v>
@@ -1257,25 +1259,25 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44028</v>
+        <v>44029</v>
       </c>
       <c r="C17" t="n">
-        <v>150319</v>
+        <v>153041</v>
       </c>
       <c r="D17" t="n">
-        <v>4047</v>
+        <v>4084</v>
       </c>
       <c r="E17" t="n">
-        <v>3983</v>
+        <v>4094</v>
       </c>
       <c r="F17" t="n">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="G17" t="n">
-        <v>4.67</v>
+        <v>4.69</v>
       </c>
       <c r="H17" t="n">
-        <v>10.64</v>
+        <v>10.76</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1284,10 +1286,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>85284</v>
+        <v>87304</v>
       </c>
       <c r="L17" t="n">
-        <v>3760</v>
+        <v>3801</v>
       </c>
       <c r="M17" t="n">
         <v>823987</v>
@@ -1359,22 +1361,22 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44028</v>
+        <v>44029</v>
       </c>
       <c r="C19" t="n">
-        <v>40829</v>
+        <v>41846</v>
       </c>
       <c r="D19" t="n">
-        <v>1332</v>
+        <v>1346</v>
       </c>
       <c r="E19" t="n">
-        <v>18838</v>
+        <v>19138</v>
       </c>
       <c r="F19" t="n">
-        <v>664</v>
+        <v>671</v>
       </c>
       <c r="G19" t="n">
-        <v>46.14</v>
+        <v>45.73</v>
       </c>
       <c r="H19" t="n">
         <v>49.85</v>
@@ -1504,20 +1506,20 @@
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C22" t="n">
-        <v>2366</v>
+        <v>2471</v>
       </c>
       <c r="D22" t="n">
         <v>37</v>
       </c>
       <c r="E22" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
-        <v>0.51</v>
+        <v>0.53</v>
       </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="b">
@@ -1696,25 +1698,25 @@
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C26" t="n">
-        <v>39344</v>
+        <v>39788</v>
       </c>
       <c r="D26" t="n">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="E26" t="n">
-        <v>1963</v>
+        <v>1981</v>
       </c>
       <c r="F26" t="n">
         <v>118</v>
       </c>
       <c r="G26" t="n">
-        <v>6.24</v>
+        <v>6.25</v>
       </c>
       <c r="H26" t="n">
-        <v>6.97</v>
+        <v>6.96</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
@@ -1723,10 +1725,10 @@
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>31452</v>
+        <v>31715</v>
       </c>
       <c r="L26" t="n">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="M26" t="n">
         <v>227938</v>
@@ -1747,10 +1749,10 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C27" t="n">
-        <v>22361</v>
+        <v>22481</v>
       </c>
       <c r="D27" t="n">
         <v>301</v>
@@ -1798,25 +1800,25 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C28" t="n">
-        <v>72410</v>
+        <v>73098</v>
       </c>
       <c r="D28" t="n">
-        <v>6024</v>
+        <v>6039</v>
       </c>
       <c r="E28" t="n">
-        <v>21120</v>
+        <v>21215</v>
       </c>
       <c r="F28" t="n">
-        <v>2401</v>
+        <v>2406</v>
       </c>
       <c r="G28" t="n">
-        <v>29.17</v>
+        <v>29.02</v>
       </c>
       <c r="H28" t="n">
-        <v>39.86</v>
+        <v>39.84</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -1845,25 +1847,25 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44028</v>
+        <v>44029</v>
       </c>
       <c r="C29" t="n">
-        <v>366164</v>
+        <v>375363</v>
       </c>
       <c r="D29" t="n">
-        <v>7475</v>
+        <v>7595</v>
       </c>
       <c r="E29" t="n">
-        <v>10199</v>
+        <v>10432</v>
       </c>
       <c r="F29" t="n">
-        <v>635</v>
+        <v>641</v>
       </c>
       <c r="G29" t="n">
-        <v>4.33</v>
+        <v>4.32</v>
       </c>
       <c r="H29" t="n">
-        <v>8.77</v>
+        <v>8.69</v>
       </c>
       <c r="I29" t="b">
         <v>0</v>
@@ -1872,10 +1874,10 @@
         <v>0</v>
       </c>
       <c r="K29" t="n">
-        <v>235539</v>
+        <v>241390</v>
       </c>
       <c r="L29" t="n">
-        <v>7243</v>
+        <v>7376</v>
       </c>
       <c r="M29" t="n">
         <v>2267875</v>
@@ -1896,25 +1898,25 @@
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C30" t="n">
-        <v>54813</v>
+        <v>55654</v>
       </c>
       <c r="D30" t="n">
-        <v>2610</v>
+        <v>2627</v>
       </c>
       <c r="E30" t="n">
-        <v>6426</v>
+        <v>6493</v>
       </c>
       <c r="F30" t="n">
         <v>373</v>
       </c>
       <c r="G30" t="n">
-        <v>11.72</v>
+        <v>11.67</v>
       </c>
       <c r="H30" t="n">
-        <v>14.29</v>
+        <v>14.2</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
@@ -1943,22 +1945,22 @@
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C31" t="n">
-        <v>1733</v>
+        <v>1795</v>
       </c>
       <c r="D31" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E31" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>1.41</v>
+        <v>1.4</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -1970,10 +1972,10 @@
         <v>1</v>
       </c>
       <c r="K31" t="n">
-        <v>2904</v>
+        <v>3010</v>
       </c>
       <c r="L31" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M31" t="n">
         <v>24129</v>
@@ -1994,25 +1996,25 @@
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C32" t="n">
-        <v>40507</v>
+        <v>41485</v>
       </c>
       <c r="D32" t="n">
-        <v>833</v>
+        <v>843</v>
       </c>
       <c r="E32" t="n">
-        <v>6620</v>
+        <v>6721</v>
       </c>
       <c r="F32" t="n">
         <v>196</v>
       </c>
       <c r="G32" t="n">
-        <v>18.08</v>
+        <v>17.93</v>
       </c>
       <c r="H32" t="n">
-        <v>23.9</v>
+        <v>23.64</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
@@ -2021,10 +2023,10 @@
         <v>1</v>
       </c>
       <c r="K32" t="n">
-        <v>36613</v>
+        <v>37485</v>
       </c>
       <c r="L32" t="n">
-        <v>820</v>
+        <v>829</v>
       </c>
       <c r="M32" t="n">
         <v>368744</v>
@@ -2045,25 +2047,25 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C33" t="n">
-        <v>135183</v>
+        <v>139872</v>
       </c>
       <c r="D33" t="n">
-        <v>3132</v>
+        <v>3168</v>
       </c>
       <c r="E33" t="n">
-        <v>35319</v>
+        <v>36504</v>
       </c>
       <c r="F33" t="n">
-        <v>1461</v>
+        <v>1470</v>
       </c>
       <c r="G33" t="n">
-        <v>26.13</v>
+        <v>26.1</v>
       </c>
       <c r="H33" t="n">
-        <v>46.65</v>
+        <v>46.4</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
@@ -2092,25 +2094,25 @@
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C34" t="n">
-        <v>45067</v>
+        <v>46026</v>
       </c>
       <c r="D34" t="n">
-        <v>1434</v>
+        <v>1444</v>
       </c>
       <c r="E34" t="n">
-        <v>1676</v>
+        <v>1690</v>
       </c>
       <c r="F34" t="n">
         <v>48</v>
       </c>
       <c r="G34" t="n">
-        <v>5.41</v>
+        <v>5.42</v>
       </c>
       <c r="H34" t="n">
-        <v>3.48</v>
+        <v>3.46</v>
       </c>
       <c r="I34" t="b">
         <v>0</v>
@@ -2119,10 +2121,10 @@
         <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>30976</v>
+        <v>31176</v>
       </c>
       <c r="L34" t="n">
-        <v>1379</v>
+        <v>1386</v>
       </c>
       <c r="M34" t="n">
         <v>269854</v>
@@ -2285,22 +2287,22 @@
         <v>44030</v>
       </c>
       <c r="C38" t="n">
-        <v>37904</v>
+        <v>38197</v>
       </c>
       <c r="D38" t="n">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="E38" t="n">
-        <v>3180</v>
+        <v>3188</v>
       </c>
       <c r="F38" t="n">
         <v>38</v>
       </c>
       <c r="G38" t="n">
-        <v>8.390000000000001</v>
+        <v>8.35</v>
       </c>
       <c r="H38" t="n">
-        <v>4.83</v>
+        <v>4.82</v>
       </c>
       <c r="I38" t="b">
         <v>1</v>
@@ -2329,25 +2331,25 @@
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C39" t="n">
-        <v>95477</v>
+        <v>97958</v>
       </c>
       <c r="D39" t="n">
-        <v>1606</v>
+        <v>1629</v>
       </c>
       <c r="E39" t="n">
-        <v>15601</v>
+        <v>15936</v>
       </c>
       <c r="F39" t="n">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="G39" t="n">
-        <v>23.95</v>
+        <v>23.89</v>
       </c>
       <c r="H39" t="n">
-        <v>32.84</v>
+        <v>32.8</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
@@ -2356,10 +2358,10 @@
         <v>1</v>
       </c>
       <c r="K39" t="n">
-        <v>65147</v>
+        <v>66695</v>
       </c>
       <c r="L39" t="n">
-        <v>1550</v>
+        <v>1573</v>
       </c>
       <c r="M39" t="n">
         <v>2179622</v>
@@ -2380,22 +2382,22 @@
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C40" t="n">
-        <v>159334</v>
+        <v>160610</v>
       </c>
       <c r="D40" t="n">
-        <v>7272</v>
+        <v>7290</v>
       </c>
       <c r="E40" t="n">
-        <v>26784</v>
+        <v>27009</v>
       </c>
       <c r="F40" t="n">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="G40" t="n">
-        <v>16.81</v>
+        <v>16.82</v>
       </c>
       <c r="H40" t="n">
         <v>27.59</v>
@@ -2427,22 +2429,22 @@
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C41" t="n">
-        <v>13752</v>
+        <v>14302</v>
       </c>
       <c r="D41" t="n">
         <v>114</v>
       </c>
       <c r="E41" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F41" t="n">
         <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>1.28</v>
+        <v>1.24</v>
       </c>
       <c r="H41" t="n">
         <v>0.88</v>
@@ -2474,25 +2476,25 @@
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C42" t="n">
-        <v>45013</v>
+        <v>45470</v>
       </c>
       <c r="D42" t="n">
-        <v>1533</v>
+        <v>1538</v>
       </c>
       <c r="E42" t="n">
-        <v>9114</v>
+        <v>9200</v>
       </c>
       <c r="F42" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G42" t="n">
-        <v>20.25</v>
+        <v>20.23</v>
       </c>
       <c r="H42" t="n">
-        <v>9.779999999999999</v>
+        <v>9.82</v>
       </c>
       <c r="I42" t="b">
         <v>1</v>
@@ -2521,19 +2523,19 @@
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C43" t="n">
-        <v>112879</v>
+        <v>113238</v>
       </c>
       <c r="D43" t="n">
-        <v>8402</v>
+        <v>8419</v>
       </c>
       <c r="E43" t="n">
-        <v>10612</v>
+        <v>10642</v>
       </c>
       <c r="F43" t="n">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="G43" t="n">
         <v>9.4</v>
@@ -2619,25 +2621,25 @@
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C45" t="n">
-        <v>31288</v>
+        <v>32246</v>
       </c>
       <c r="D45" t="n">
-        <v>1121</v>
+        <v>1130</v>
       </c>
       <c r="E45" t="n">
-        <v>6910</v>
+        <v>7584</v>
       </c>
       <c r="F45" t="n">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="G45" t="n">
-        <v>34.6</v>
+        <v>32.77</v>
       </c>
       <c r="H45" t="n">
-        <v>36.82</v>
+        <v>36.09</v>
       </c>
       <c r="I45" t="b">
         <v>0</v>
@@ -2646,10 +2648,10 @@
         <v>1</v>
       </c>
       <c r="K45" t="n">
-        <v>19970</v>
+        <v>23144</v>
       </c>
       <c r="L45" t="n">
-        <v>1013</v>
+        <v>1053</v>
       </c>
       <c r="M45" t="n">
         <v>704896</v>

</xml_diff>

<commit_message>
Results from July 18, 2020 08:22:23 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-18.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-18.xlsx
@@ -2287,19 +2287,19 @@
         <v>44030</v>
       </c>
       <c r="C38" t="n">
-        <v>38197</v>
+        <v>38259</v>
       </c>
       <c r="D38" t="n">
         <v>789</v>
       </c>
       <c r="E38" t="n">
-        <v>3188</v>
+        <v>3189</v>
       </c>
       <c r="F38" t="n">
         <v>38</v>
       </c>
       <c r="G38" t="n">
-        <v>8.35</v>
+        <v>8.34</v>
       </c>
       <c r="H38" t="n">
         <v>4.82</v>

</xml_diff>